<commit_message>
Correct "Ogiso" in S00050 lol
</commit_message>
<xml_diff>
--- a/tl/S00050.MES.BIN.xlsx
+++ b/tl/S00050.MES.BIN.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B777F51-A4AA-4B16-A46B-B97C7570EB85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F9F32D8-676F-41DD-9F6E-5CA909D67E7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2820" yWindow="9810" windowWidth="45900" windowHeight="19845" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2820" yWindow="19005" windowWidth="54585" windowHeight="12600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="S00050.MES.BIN" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1840" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="920" uniqueCount="232">
   <si>
     <t>Status</t>
   </si>
@@ -53,262 +53,268 @@
     <t>3</t>
   </si>
   <si>
+    <t>Floor Director</t>
+  </si>
+  <si>
+    <t>Heeey, Fujii-kun. Hey!"</t>
+  </si>
+  <si>
+    <t>The FD (Floor Director) is calling.</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>I wonder what it could be?</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>Usually they call me '&lt;RBaito|part-timer&gt;', but this time it's 'Fujii-kun'.</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>Touya</t>
+  </si>
+  <si>
+    <t>What is it?"</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>The FD has a slightly unpleasant look on his face.</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>"I'm pretty sure you're friends with Morikawa, right, Fujii-kun?"</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>"Um, well..."</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>It's unusual for someone from the company to talk about private matters.</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>"You see, it looks like Morikawa left the earrings she's going to wear on stage in the dressing room today."</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>Morikawa-san and the manager are currently too busy doing the final check."</t>
+  </si>
+  <si>
+    <t>Not sure why -san is only on this line.</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>Right...</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>I heard they're in her bag. Sorry to ask, but could you go get them for me? You should be able to recognize Morikawa's belongings, right?"</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>Yeah, probably..."</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>Sorry again, but could you go and get them quickly? I heard the earrings are easy to spot."</t>
+  </si>
+  <si>
+    <t>31</t>
+  </si>
+  <si>
+    <t>Oh, I also need to go back to the final check soon. Alright, hurry back."</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>His shoes make loud sounds as he walk back to the stage.</t>
+  </si>
+  <si>
+    <t>He then makes loud slipper noises and returns to the stage.</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>It can't be helped. I quickly head for the dressing room.</t>
+  </si>
+  <si>
+    <t>No choice. I quickly heads for the dressing room.</t>
+  </si>
+  <si>
+    <t>37</t>
+  </si>
+  <si>
+    <t>The dressing room follows strict rules like "let's keep it clean for everyone" that make it feel like a elementary school, but the white walls remain spotless and it is an uncommonly clean space within the station.</t>
+  </si>
+  <si>
+    <t>The waiting room was strictly upholding the rules like, "Let's use it nicely, everyone," like an elementary school, and it was a rare clean space within the station, with white walls still white.</t>
+  </si>
+  <si>
+    <t>39</t>
+  </si>
+  <si>
+    <t>Let's see… Where is Yuki's bag?</t>
+  </si>
+  <si>
+    <t>41</t>
+  </si>
+  <si>
+    <t>Oh, there it is.</t>
+  </si>
+  <si>
+    <t>43</t>
+  </si>
+  <si>
+    <t>A cloth bag is placed on the corner of the couch. Inside it is a faint pink pouch.</t>
+  </si>
+  <si>
+    <t>A cloth bag is placed in the corner of the long chair. There was a faint pink pouch inside.</t>
+  </si>
+  <si>
+    <t>45</t>
+  </si>
+  <si>
+    <t>Probably inside this...</t>
+  </si>
+  <si>
+    <t>47</t>
+  </si>
+  <si>
+    <t>...There they are.</t>
+  </si>
+  <si>
+    <t>49</t>
+  </si>
+  <si>
+    <t>I suppose even such a small accessory is very important to a pro.</t>
+  </si>
+  <si>
+    <t>I suppose even such a small accessory is very important to an expert.</t>
+  </si>
+  <si>
+    <t>51</t>
+  </si>
+  <si>
+    <t>I can't say I understand, but I have to hurry and return them anyway.</t>
+  </si>
+  <si>
+    <t>I can't say I understand, but I have to hurry and get it anyway.</t>
+  </si>
+  <si>
+    <t>53</t>
+  </si>
+  <si>
+    <t>Something catches my attention as I'm about to leave though.</t>
+  </si>
+  <si>
+    <t>Then, as I'm about to leave,</t>
+  </si>
+  <si>
+    <t>55</t>
+  </si>
+  <si>
+    <t>What's this? Someone has left their notebook on the table.</t>
+  </si>
+  <si>
+    <t>Oh no...Someone has left their notebook on the table.</t>
+  </si>
+  <si>
+    <t>57</t>
+  </si>
+  <si>
+    <t>Whose could it be?</t>
+  </si>
+  <si>
+    <t>59</t>
+  </si>
+  <si>
+    <t>I'll take a closer look.</t>
+  </si>
+  <si>
+    <t>Let me take a look.</t>
+  </si>
+  <si>
+    <t>61</t>
+  </si>
+  <si>
+    <t>No, it's not a notebook.</t>
+  </si>
+  <si>
+    <t>63</t>
+  </si>
+  <si>
+    <t>Rather, it's a novel with an elegant leather book cover.</t>
+  </si>
+  <si>
+    <t>65</t>
+  </si>
+  <si>
+    <t>It's not Yuki's...</t>
+  </si>
+  <si>
+    <t>I don't think this is Yuki's...</t>
+  </si>
+  <si>
+    <t>67</t>
+  </si>
+  <si>
+    <t>She wouldn't have something like this, I don't think?</t>
+  </si>
+  <si>
+    <t>At least, I don't think she has one like this.</t>
+  </si>
+  <si>
+    <t>69</t>
+  </si>
+  <si>
+    <t>At that moment, the door opens and someone enters the room.</t>
+  </si>
+  <si>
+    <t>71</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
     <t>Rina</t>
   </si>
   <si>
-    <t>Heeey, Fujii-kun. Hey!"</t>
-  </si>
-  <si>
-    <t>The FD (Floor Director) is calling.</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>I wonder what it could be?</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>Usually they call me '&lt;RBaito|part-timer&gt;', but this time it's 'Fujii-kun'.</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>Touya</t>
-  </si>
-  <si>
-    <t>What is it?"</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>The FD has a slightly unpleasant look on his face.</t>
-  </si>
-  <si>
-    <t>13</t>
-  </si>
-  <si>
-    <t>"I'm pretty sure you're friends with Morikawa, right, Fujii-kun?"</t>
-  </si>
-  <si>
-    <t>15</t>
-  </si>
-  <si>
-    <t>"Um, well..."</t>
-  </si>
-  <si>
-    <t>17</t>
-  </si>
-  <si>
-    <t>It's unusual for someone from the company to talk about private matters.</t>
-  </si>
-  <si>
-    <t>19</t>
-  </si>
-  <si>
-    <t>"You see, it looks like Morikawa left the earrings she's going to wear on stage in the dressing room today."</t>
-  </si>
-  <si>
-    <t>21</t>
-  </si>
-  <si>
-    <t>Morikawa-san and the manager are currently too busy doing the final check."</t>
-  </si>
-  <si>
-    <t>Not sure why -san is only on this line.</t>
-  </si>
-  <si>
-    <t>23</t>
-  </si>
-  <si>
-    <t>Right...</t>
-  </si>
-  <si>
-    <t>25</t>
-  </si>
-  <si>
-    <t>I heard they're in her bag. Sorry to ask, but could you go get them for me? You should be able to recognize Morikawa's belongings, right?"</t>
-  </si>
-  <si>
-    <t>27</t>
-  </si>
-  <si>
-    <t>Yeah, probably..."</t>
-  </si>
-  <si>
-    <t>29</t>
-  </si>
-  <si>
-    <t>Sorry again, but could you go and get them quickly? I heard the earrings are easy to spot."</t>
-  </si>
-  <si>
-    <t>31</t>
-  </si>
-  <si>
-    <t>Oh, I also need to go back to the final check soon. Alright, hurry back."</t>
-  </si>
-  <si>
-    <t>33</t>
-  </si>
-  <si>
-    <t>His shoes make loud sounds as he walk back to the stage.</t>
-  </si>
-  <si>
-    <t>He then makes loud slipper noises and returns to the stage.</t>
-  </si>
-  <si>
-    <t>35</t>
-  </si>
-  <si>
-    <t>It can't be helped. I quickly head for the dressing room.</t>
-  </si>
-  <si>
-    <t>No choice. I quickly heads for the dressing room.</t>
-  </si>
-  <si>
-    <t>37</t>
-  </si>
-  <si>
-    <t>The waiting room was strictly upholding the rules like, "Let's use it nicely, everyone," like an elementary school, and it was a rare clean space within the station, with white walls still white.</t>
-  </si>
-  <si>
-    <t>39</t>
-  </si>
-  <si>
-    <t>Let's see… Where is Yuki's bag?</t>
-  </si>
-  <si>
-    <t>41</t>
-  </si>
-  <si>
-    <t>Oh, there it is.</t>
-  </si>
-  <si>
-    <t>43</t>
-  </si>
-  <si>
-    <t>A cloth bag is placed on the corner of the couch. Inside it is a faint pink pouch.</t>
-  </si>
-  <si>
-    <t>A cloth bag is placed in the corner of the long chair. There was a faint pink pouch inside.</t>
-  </si>
-  <si>
-    <t>45</t>
-  </si>
-  <si>
-    <t>Probably inside this...</t>
-  </si>
-  <si>
-    <t>47</t>
-  </si>
-  <si>
-    <t>...There they are.</t>
-  </si>
-  <si>
-    <t>49</t>
-  </si>
-  <si>
-    <t>I suppose even such a small accessory is very important to a pro.</t>
-  </si>
-  <si>
-    <t>I suppose even such a small accessory is very important to an expert.</t>
-  </si>
-  <si>
-    <t>51</t>
-  </si>
-  <si>
-    <t>I can't say I understand, but I have to hurry and return them anyway.</t>
-  </si>
-  <si>
-    <t>I can't say I understand, but I have to hurry and get it anyway.</t>
-  </si>
-  <si>
-    <t>53</t>
-  </si>
-  <si>
-    <t>Something catches my attention as I'm about to leave though.</t>
-  </si>
-  <si>
-    <t>Then, as I'm about to leave,</t>
-  </si>
-  <si>
-    <t>55</t>
-  </si>
-  <si>
-    <t>What's this? Someone has left their notebook on the table.</t>
-  </si>
-  <si>
-    <t>Oh no...Someone has left their notebook on the table.</t>
-  </si>
-  <si>
-    <t>57</t>
-  </si>
-  <si>
-    <t>Whose could it be?</t>
-  </si>
-  <si>
-    <t>59</t>
-  </si>
-  <si>
-    <t>I'll take a closer look.</t>
-  </si>
-  <si>
-    <t>Let me take a look.</t>
-  </si>
-  <si>
-    <t>61</t>
-  </si>
-  <si>
-    <t>No, it's not a notebook.</t>
-  </si>
-  <si>
-    <t>63</t>
-  </si>
-  <si>
-    <t>Rather, it's a novel with an elegant leather book cover.</t>
-  </si>
-  <si>
-    <t>65</t>
-  </si>
-  <si>
-    <t>It's not Yuki's...</t>
-  </si>
-  <si>
-    <t>I don't think this is Yuki's...</t>
-  </si>
-  <si>
-    <t>67</t>
-  </si>
-  <si>
-    <t>She wouldn't have something like this, I don't think?</t>
-  </si>
-  <si>
-    <t>At least, I don't think she has one like this.</t>
-  </si>
-  <si>
-    <t>69</t>
-  </si>
-  <si>
-    <t>At that moment, the door opens and someone enters the room.</t>
-  </si>
-  <si>
-    <t>71</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
     <t>Oh?</t>
   </si>
   <si>
     <t>73</t>
   </si>
   <si>
-    <t>It's Rina Ogiso, who lets out a surprised sound upon seeing me.</t>
+    <t>It's Rina Ogata, who lets out a surprised sound upon seeing me.</t>
   </si>
   <si>
     <t>The one who makes a surprised sound is Rina Ogiso.</t>
@@ -431,13 +437,13 @@
     <t>109</t>
   </si>
   <si>
-    <t>Rina-chan...&lt;Rright|ですか&gt;?</t>
+    <t>Rina-chan...&lt;Ris it|ですか&gt;?</t>
   </si>
   <si>
     <t>111</t>
   </si>
   <si>
-    <t>"What do you mean "&lt;Rright|ですか&gt;"?</t>
+    <t>"What do you mean "&lt;Ris it|ですか&gt;"?</t>
   </si>
   <si>
     <t>113</t>
@@ -705,9 +711,6 @@
   </si>
   <si>
     <t>Don't read many books</t>
-  </si>
-  <si>
-    <t>The dressing room follows strict rules like "let's keep it clean for everyone" that make it feel like an elementary school, but the white walls remain spotless and it is an uncommonly clean space within the station.</t>
   </si>
 </sst>
 </file>
@@ -1130,7 +1133,7 @@
   <dimension ref="A1:J92"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1766,10 +1769,10 @@
         <v>9</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>230</v>
+        <v>52</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H20" s="3" t="s">
         <v>9</v>
@@ -1786,7 +1789,7 @@
         <v>9</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>9</v>
@@ -1801,7 +1804,7 @@
         <v>9</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H21" s="5" t="s">
         <v>9</v>
@@ -1818,7 +1821,7 @@
         <v>9</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>9</v>
@@ -1833,7 +1836,7 @@
         <v>9</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H22" s="3" t="s">
         <v>9</v>
@@ -1850,7 +1853,7 @@
         <v>9</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>9</v>
@@ -1862,10 +1865,10 @@
         <v>9</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H23" s="5" t="s">
         <v>9</v>
@@ -1882,7 +1885,7 @@
         <v>9</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>9</v>
@@ -1897,7 +1900,7 @@
         <v>9</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H24" s="3" t="s">
         <v>9</v>
@@ -1914,7 +1917,7 @@
         <v>9</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>9</v>
@@ -1929,7 +1932,7 @@
         <v>9</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H25" s="5" t="s">
         <v>9</v>
@@ -1946,7 +1949,7 @@
         <v>9</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>9</v>
@@ -1958,10 +1961,10 @@
         <v>9</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="H26" s="3" t="s">
         <v>9</v>
@@ -1978,7 +1981,7 @@
         <v>9</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>9</v>
@@ -1990,10 +1993,10 @@
         <v>9</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H27" s="5" t="s">
         <v>9</v>
@@ -2010,7 +2013,7 @@
         <v>9</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>9</v>
@@ -2022,10 +2025,10 @@
         <v>9</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H28" s="3" t="s">
         <v>9</v>
@@ -2042,7 +2045,7 @@
         <v>9</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>9</v>
@@ -2054,10 +2057,10 @@
         <v>9</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H29" s="5" t="s">
         <v>9</v>
@@ -2074,7 +2077,7 @@
         <v>9</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>9</v>
@@ -2089,7 +2092,7 @@
         <v>9</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H30" s="3" t="s">
         <v>9</v>
@@ -2106,7 +2109,7 @@
         <v>9</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>9</v>
@@ -2118,10 +2121,10 @@
         <v>9</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H31" s="5" t="s">
         <v>9</v>
@@ -2138,7 +2141,7 @@
         <v>9</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>9</v>
@@ -2153,7 +2156,7 @@
         <v>9</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H32" s="3" t="s">
         <v>9</v>
@@ -2170,7 +2173,7 @@
         <v>9</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>9</v>
@@ -2185,7 +2188,7 @@
         <v>9</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H33" s="5" t="s">
         <v>9</v>
@@ -2202,7 +2205,7 @@
         <v>9</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>9</v>
@@ -2214,10 +2217,10 @@
         <v>9</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H34" s="3" t="s">
         <v>9</v>
@@ -2234,7 +2237,7 @@
         <v>9</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>9</v>
@@ -2246,10 +2249,10 @@
         <v>9</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H35" s="5" t="s">
         <v>9</v>
@@ -2266,7 +2269,7 @@
         <v>9</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>9</v>
@@ -2281,7 +2284,7 @@
         <v>9</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H36" s="3" t="s">
         <v>9</v>
@@ -2298,13 +2301,13 @@
         <v>9</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>12</v>
+        <v>96</v>
       </c>
       <c r="E37" s="4" t="s">
         <v>9</v>
@@ -2313,7 +2316,7 @@
         <v>9</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="H37" s="5" t="s">
         <v>9</v>
@@ -2330,7 +2333,7 @@
         <v>9</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>9</v>
@@ -2342,10 +2345,10 @@
         <v>9</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="H38" s="3" t="s">
         <v>9</v>
@@ -2362,7 +2365,7 @@
         <v>9</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C39" s="4" t="s">
         <v>9</v>
@@ -2377,7 +2380,7 @@
         <v>9</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="H39" s="5" t="s">
         <v>9</v>
@@ -2394,7 +2397,7 @@
         <v>9</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>9</v>
@@ -2409,7 +2412,7 @@
         <v>9</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="H40" s="3" t="s">
         <v>9</v>
@@ -2426,22 +2429,22 @@
         <v>9</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>12</v>
+        <v>96</v>
       </c>
       <c r="E41" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="H41" s="5" t="s">
         <v>9</v>
@@ -2458,7 +2461,7 @@
         <v>9</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>10</v>
@@ -2470,10 +2473,10 @@
         <v>9</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="H42" s="3" t="s">
         <v>9</v>
@@ -2490,7 +2493,7 @@
         <v>9</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="C43" s="4" t="s">
         <v>9</v>
@@ -2505,7 +2508,7 @@
         <v>9</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="H43" s="5" t="s">
         <v>9</v>
@@ -2522,13 +2525,13 @@
         <v>9</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>12</v>
+        <v>96</v>
       </c>
       <c r="E44" s="2" t="s">
         <v>9</v>
@@ -2537,7 +2540,7 @@
         <v>9</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="H44" s="3" t="s">
         <v>9</v>
@@ -2554,7 +2557,7 @@
         <v>9</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C45" s="4" t="s">
         <v>9</v>
@@ -2569,7 +2572,7 @@
         <v>9</v>
       </c>
       <c r="G45" s="5" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="H45" s="5" t="s">
         <v>9</v>
@@ -2586,7 +2589,7 @@
         <v>9</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>9</v>
@@ -2601,7 +2604,7 @@
         <v>9</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="H46" s="3" t="s">
         <v>9</v>
@@ -2618,7 +2621,7 @@
         <v>9</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="C47" s="4" t="s">
         <v>9</v>
@@ -2633,7 +2636,7 @@
         <v>9</v>
       </c>
       <c r="G47" s="5" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="H47" s="5" t="s">
         <v>9</v>
@@ -2650,22 +2653,22 @@
         <v>9</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>12</v>
+        <v>96</v>
       </c>
       <c r="E48" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="H48" s="3" t="s">
         <v>9</v>
@@ -2682,7 +2685,7 @@
         <v>9</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="C49" s="4" t="s">
         <v>10</v>
@@ -2697,7 +2700,7 @@
         <v>9</v>
       </c>
       <c r="G49" s="5" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="H49" s="5" t="s">
         <v>9</v>
@@ -2714,13 +2717,13 @@
         <v>9</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>12</v>
+        <v>96</v>
       </c>
       <c r="E50" s="2" t="s">
         <v>9</v>
@@ -2729,7 +2732,7 @@
         <v>9</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="H50" s="3" t="s">
         <v>9</v>
@@ -2746,7 +2749,7 @@
         <v>9</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="C51" s="4" t="s">
         <v>10</v>
@@ -2761,7 +2764,7 @@
         <v>9</v>
       </c>
       <c r="G51" s="5" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="H51" s="5" t="s">
         <v>9</v>
@@ -2778,22 +2781,22 @@
         <v>9</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>12</v>
+        <v>96</v>
       </c>
       <c r="E52" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="H52" s="3" t="s">
         <v>9</v>
@@ -2810,7 +2813,7 @@
         <v>9</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C53" s="4" t="s">
         <v>10</v>
@@ -2825,7 +2828,7 @@
         <v>9</v>
       </c>
       <c r="G53" s="5" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="H53" s="5" t="s">
         <v>9</v>
@@ -2842,13 +2845,13 @@
         <v>9</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>12</v>
+        <v>96</v>
       </c>
       <c r="E54" s="2" t="s">
         <v>9</v>
@@ -2857,7 +2860,7 @@
         <v>9</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="H54" s="3" t="s">
         <v>9</v>
@@ -2874,13 +2877,13 @@
         <v>9</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>12</v>
+        <v>96</v>
       </c>
       <c r="E55" s="4" t="s">
         <v>9</v>
@@ -2889,7 +2892,7 @@
         <v>9</v>
       </c>
       <c r="G55" s="5" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="H55" s="5" t="s">
         <v>9</v>
@@ -2906,7 +2909,7 @@
         <v>9</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>10</v>
@@ -2921,7 +2924,7 @@
         <v>9</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="H56" s="3" t="s">
         <v>9</v>
@@ -2938,13 +2941,13 @@
         <v>9</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>12</v>
+        <v>96</v>
       </c>
       <c r="E57" s="4" t="s">
         <v>9</v>
@@ -2953,7 +2956,7 @@
         <v>9</v>
       </c>
       <c r="G57" s="5" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="H57" s="5" t="s">
         <v>9</v>
@@ -2970,7 +2973,7 @@
         <v>9</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>10</v>
@@ -2985,7 +2988,7 @@
         <v>9</v>
       </c>
       <c r="G58" s="3" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="H58" s="3" t="s">
         <v>9</v>
@@ -3002,22 +3005,22 @@
         <v>9</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>12</v>
+        <v>96</v>
       </c>
       <c r="E59" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F59" s="4" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="G59" s="5" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="H59" s="5" t="s">
         <v>9</v>
@@ -3034,7 +3037,7 @@
         <v>9</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="C60" s="2" t="s">
         <v>10</v>
@@ -3049,7 +3052,7 @@
         <v>36</v>
       </c>
       <c r="G60" s="3" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="H60" s="3" t="s">
         <v>9</v>
@@ -3066,13 +3069,13 @@
         <v>9</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>12</v>
+        <v>96</v>
       </c>
       <c r="E61" s="4" t="s">
         <v>9</v>
@@ -3081,7 +3084,7 @@
         <v>9</v>
       </c>
       <c r="G61" s="5" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="H61" s="5" t="s">
         <v>9</v>
@@ -3098,7 +3101,7 @@
         <v>9</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="C62" s="2" t="s">
         <v>9</v>
@@ -3113,7 +3116,7 @@
         <v>9</v>
       </c>
       <c r="G62" s="3" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="H62" s="3" t="s">
         <v>9</v>
@@ -3130,22 +3133,22 @@
         <v>9</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>12</v>
+        <v>96</v>
       </c>
       <c r="E63" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F63" s="4" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="G63" s="5" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="H63" s="5" t="s">
         <v>9</v>
@@ -3162,7 +3165,7 @@
         <v>9</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="C64" s="2" t="s">
         <v>9</v>
@@ -3177,7 +3180,7 @@
         <v>9</v>
       </c>
       <c r="G64" s="3" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="H64" s="3" t="s">
         <v>9</v>
@@ -3194,22 +3197,22 @@
         <v>9</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>12</v>
+        <v>96</v>
       </c>
       <c r="E65" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F65" s="4" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="G65" s="5" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="H65" s="5" t="s">
         <v>9</v>
@@ -3226,7 +3229,7 @@
         <v>9</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="C66" s="2" t="s">
         <v>9</v>
@@ -3238,10 +3241,10 @@
         <v>9</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="G66" s="3" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="H66" s="3" t="s">
         <v>9</v>
@@ -3258,7 +3261,7 @@
         <v>9</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="C67" s="4" t="s">
         <v>9</v>
@@ -3270,10 +3273,10 @@
         <v>9</v>
       </c>
       <c r="F67" s="4" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="G67" s="5" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="H67" s="5" t="s">
         <v>9</v>
@@ -3290,22 +3293,22 @@
         <v>9</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>12</v>
+        <v>96</v>
       </c>
       <c r="E68" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="G68" s="3" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="H68" s="3" t="s">
         <v>9</v>
@@ -3322,22 +3325,22 @@
         <v>9</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D69" s="4" t="s">
-        <v>12</v>
+        <v>96</v>
       </c>
       <c r="E69" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F69" s="4" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="G69" s="5" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="H69" s="5" t="s">
         <v>9</v>
@@ -3354,7 +3357,7 @@
         <v>9</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="C70" s="2" t="s">
         <v>10</v>
@@ -3366,10 +3369,10 @@
         <v>9</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="G70" s="3" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="H70" s="3" t="s">
         <v>9</v>
@@ -3386,7 +3389,7 @@
         <v>9</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="C71" s="4" t="s">
         <v>9</v>
@@ -3401,7 +3404,7 @@
         <v>9</v>
       </c>
       <c r="G71" s="5" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="H71" s="5" t="s">
         <v>9</v>
@@ -3418,22 +3421,22 @@
         <v>9</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>12</v>
+        <v>96</v>
       </c>
       <c r="E72" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="G72" s="3" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="H72" s="3" t="s">
         <v>9</v>
@@ -3450,7 +3453,7 @@
         <v>9</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="C73" s="4" t="s">
         <v>9</v>
@@ -3465,7 +3468,7 @@
         <v>9</v>
       </c>
       <c r="G73" s="5" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="H73" s="5" t="s">
         <v>9</v>
@@ -3482,7 +3485,7 @@
         <v>9</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="C74" s="2" t="s">
         <v>10</v>
@@ -3497,7 +3500,7 @@
         <v>9</v>
       </c>
       <c r="G74" s="3" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="H74" s="3" t="s">
         <v>9</v>
@@ -3514,7 +3517,7 @@
         <v>9</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="C75" s="4" t="s">
         <v>9</v>
@@ -3526,10 +3529,10 @@
         <v>9</v>
       </c>
       <c r="F75" s="4" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="G75" s="5" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="H75" s="5" t="s">
         <v>9</v>
@@ -3546,7 +3549,7 @@
         <v>9</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="C76" s="2" t="s">
         <v>9</v>
@@ -3558,10 +3561,10 @@
         <v>9</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="G76" s="3" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="H76" s="3" t="s">
         <v>9</v>
@@ -3578,7 +3581,7 @@
         <v>9</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="C77" s="4" t="s">
         <v>10</v>
@@ -3590,10 +3593,10 @@
         <v>9</v>
       </c>
       <c r="F77" s="4" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="G77" s="5" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="H77" s="5" t="s">
         <v>9</v>
@@ -3610,7 +3613,7 @@
         <v>9</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="C78" s="2" t="s">
         <v>9</v>
@@ -3625,7 +3628,7 @@
         <v>9</v>
       </c>
       <c r="G78" s="3" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="H78" s="3" t="s">
         <v>9</v>
@@ -3642,7 +3645,7 @@
         <v>9</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="C79" s="4" t="s">
         <v>9</v>
@@ -3657,7 +3660,7 @@
         <v>9</v>
       </c>
       <c r="G79" s="5" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="H79" s="5" t="s">
         <v>9</v>
@@ -3674,22 +3677,22 @@
         <v>9</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>12</v>
+        <v>96</v>
       </c>
       <c r="E80" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="G80" s="3" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="H80" s="3" t="s">
         <v>9</v>
@@ -3706,7 +3709,7 @@
         <v>9</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="C81" s="4" t="s">
         <v>10</v>
@@ -3718,10 +3721,10 @@
         <v>9</v>
       </c>
       <c r="F81" s="4" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="G81" s="5" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="H81" s="5" t="s">
         <v>9</v>
@@ -3738,7 +3741,7 @@
         <v>9</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="C82" s="2" t="s">
         <v>9</v>
@@ -3753,7 +3756,7 @@
         <v>9</v>
       </c>
       <c r="G82" s="3" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="H82" s="3" t="s">
         <v>9</v>
@@ -3770,7 +3773,7 @@
         <v>9</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="C83" s="4" t="s">
         <v>9</v>
@@ -3785,7 +3788,7 @@
         <v>9</v>
       </c>
       <c r="G83" s="5" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="H83" s="5" t="s">
         <v>9</v>
@@ -3802,13 +3805,13 @@
         <v>9</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>12</v>
+        <v>96</v>
       </c>
       <c r="E84" s="2" t="s">
         <v>9</v>
@@ -3817,7 +3820,7 @@
         <v>9</v>
       </c>
       <c r="G84" s="3" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="H84" s="3" t="s">
         <v>9</v>
@@ -3834,7 +3837,7 @@
         <v>9</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="C85" s="4" t="s">
         <v>9</v>
@@ -3849,7 +3852,7 @@
         <v>9</v>
       </c>
       <c r="G85" s="5" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="H85" s="5" t="s">
         <v>9</v>
@@ -3866,13 +3869,13 @@
         <v>9</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>12</v>
+        <v>96</v>
       </c>
       <c r="E86" s="2" t="s">
         <v>9</v>
@@ -3881,7 +3884,7 @@
         <v>9</v>
       </c>
       <c r="G86" s="3" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="H86" s="3" t="s">
         <v>9</v>
@@ -3898,7 +3901,7 @@
         <v>9</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="C87" s="4" t="s">
         <v>10</v>
@@ -3913,7 +3916,7 @@
         <v>9</v>
       </c>
       <c r="G87" s="5" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="H87" s="5" t="s">
         <v>9</v>
@@ -3930,25 +3933,25 @@
         <v>9</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>12</v>
+        <v>96</v>
       </c>
       <c r="E88" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="G88" s="3" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="H88" s="3" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="I88" s="3" t="s">
         <v>9</v>
@@ -3962,7 +3965,7 @@
         <v>9</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="C89" s="4" t="s">
         <v>9</v>
@@ -3974,10 +3977,10 @@
         <v>9</v>
       </c>
       <c r="F89" s="4" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="G89" s="5" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="H89" s="5" t="s">
         <v>9</v>
@@ -3994,7 +3997,7 @@
         <v>9</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="C90" s="2" t="s">
         <v>9</v>
@@ -4006,10 +4009,10 @@
         <v>9</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="G90" s="3" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="H90" s="3" t="s">
         <v>9</v>
@@ -4026,7 +4029,7 @@
         <v>9</v>
       </c>
       <c r="B91" s="4" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="C91" s="4" t="s">
         <v>9</v>
@@ -4038,10 +4041,10 @@
         <v>9</v>
       </c>
       <c r="F91" s="4" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="G91" s="5" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="H91" s="5" t="s">
         <v>9</v>
@@ -4058,7 +4061,7 @@
         <v>9</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="C92" s="2" t="s">
         <v>9</v>
@@ -4070,10 +4073,10 @@
         <v>9</v>
       </c>
       <c r="F92" s="2" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="G92" s="3" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="H92" s="3" t="s">
         <v>9</v>

</xml_diff>